<commit_message>
Lab file - preview summary
</commit_message>
<xml_diff>
--- a/app/assets/images/LabFilesReceived_FFO_20220113_62010_SLF_File1.xlsx
+++ b/app/assets/images/LabFilesReceived_FFO_20220113_62010_SLF_File1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chris.houlden/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE5E99B8-9B1E-0C41-9FAD-F2F7B91AD610}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{F32B02D9-CB6D-3E48-9CF6-C1FCE470EE0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-25260" yWindow="-3580" windowWidth="15960" windowHeight="17500" firstSheet="3" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
     <sheet name="Total non-hits" sheetId="4" r:id="rId4"/>
     <sheet name="Total rejections (errors)" sheetId="5" r:id="rId5"/>
     <sheet name="Total rejections (policy)" sheetId="6" r:id="rId6"/>
-    <sheet name="Cloned results" sheetId="12" r:id="rId7"/>
+    <sheet name="Re-issued results" sheetId="12" r:id="rId7"/>
     <sheet name="Rejections outstanding" sheetId="7" r:id="rId8"/>
     <sheet name="Checked manual matches" sheetId="8" r:id="rId9"/>
     <sheet name="Checked dummy registrations" sheetId="9" r:id="rId10"/>
@@ -285,7 +285,7 @@
     <t>Checked rejected results resolved</t>
   </si>
   <si>
-    <t>Cloned results</t>
+    <t>Re-issued results</t>
   </si>
 </sst>
 </file>
@@ -353,7 +353,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
@@ -389,6 +389,9 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1551,8 +1554,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R10"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="16" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -4725,8 +4728,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{145131A8-8C54-3B47-BD1F-71B369285067}">
   <dimension ref="A1:K3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4747,8 +4750,8 @@
       <c r="K1" s="3"/>
     </row>
     <row r="2" spans="1:11" s="1" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="12" t="s">
-        <v>49</v>
+      <c r="A2" s="17" t="s">
+        <v>84</v>
       </c>
       <c r="B2" s="13"/>
       <c r="C2" s="13"/>

</xml_diff>